<commit_message>
Added weights binary files creation using python. Small preparations for ap_fixed, still doing Seg.Fault if not using float which might get fixed when using binary files for the weights.
</commit_message>
<xml_diff>
--- a/documents/HLS_microfaune_stats.xlsx
+++ b/documents/HLS_microfaune_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rodrigo\ISEL\2_Mestrado\2-ANO_1-sem\TFM\BAD_FPGA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C139FF84-E3E4-4774-A70C-761C4492F0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20079401-4312-43B6-84D8-CEF3999C9342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="915" windowWidth="24825" windowHeight="12945" firstSheet="3" activeTab="10" xr2:uid="{120B1578-28CF-4120-A86D-E8475CFEE8FD}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{120B1578-28CF-4120-A86D-E8475CFEE8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="80">
   <si>
     <t>HLS - microfaune_ai</t>
   </si>
@@ -274,6 +274,21 @@
   </si>
   <si>
     <t>baseline in HLS + reordered gru weights, pipelined gru</t>
+  </si>
+  <si>
+    <t>GitHub commit</t>
+  </si>
+  <si>
+    <t>ebb4c34a68f2eb1e245302e9664efb0fe581c014</t>
+  </si>
+  <si>
+    <t>b7f51ec62093258946e514e9b10ab0e6b0e360d7</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -309,8 +324,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,29 +641,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8BB9F6-F232-448E-BA7F-3C1C034E3083}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>15</v>
       </c>
@@ -666,8 +684,11 @@
       <c r="N4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -695,8 +716,14 @@
       <c r="N5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -721,8 +748,14 @@
       <c r="N6">
         <v>169128</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>45103.056006944447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -746,6 +779,12 @@
       </c>
       <c r="N7">
         <v>118063</v>
+      </c>
+      <c r="P7" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>45115.812395833331</v>
       </c>
     </row>
   </sheetData>
@@ -1338,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D80ED4-AEBE-471E-86CF-5C682FAEBE3C}">
   <dimension ref="A1:AO9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Load weights for test_bench from binary files.
</commit_message>
<xml_diff>
--- a/documents/HLS_microfaune_stats.xlsx
+++ b/documents/HLS_microfaune_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rodrigo\ISEL\2_Mestrado\2-ANO_1-sem\TFM\BAD_FPGA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20079401-4312-43B6-84D8-CEF3999C9342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70B5FE5-A730-4552-848A-253D3F56A0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{120B1578-28CF-4120-A86D-E8475CFEE8FD}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="84">
   <si>
     <t>HLS - microfaune_ai</t>
   </si>
@@ -289,6 +289,18 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>all with ap_fixed&lt;16,7&gt;</t>
+  </si>
+  <si>
+    <t>predict no ints</t>
+  </si>
+  <si>
+    <t>predict cycles no longer use ints, weights require loading</t>
+  </si>
+  <si>
+    <t>results are wrong, only to explore the hw resources</t>
   </si>
 </sst>
 </file>
@@ -641,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8BB9F6-F232-448E-BA7F-3C1C034E3083}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -660,131 +672,184 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" t="s">
         <v>5</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L6" t="s">
         <v>65</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M6" t="s">
         <v>66</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N6" t="s">
         <v>67</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P6" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6">
-        <v>656364844</v>
-      </c>
-      <c r="K6">
-        <v>15724</v>
-      </c>
-      <c r="L6">
-        <v>970</v>
-      </c>
-      <c r="M6">
-        <v>116953</v>
-      </c>
-      <c r="N6">
-        <v>169128</v>
-      </c>
-      <c r="P6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>45103.056006944447</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>656364844</v>
+      </c>
+      <c r="K8">
+        <v>15724</v>
+      </c>
+      <c r="L8">
+        <v>970</v>
+      </c>
+      <c r="M8">
+        <v>116953</v>
+      </c>
+      <c r="N8">
+        <v>169128</v>
+      </c>
+      <c r="P8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>45103.056006944447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7">
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9">
         <v>448215980</v>
       </c>
-      <c r="K7">
+      <c r="K9">
         <v>11508</v>
       </c>
-      <c r="L7">
+      <c r="L9">
         <v>340</v>
       </c>
-      <c r="M7">
+      <c r="M9">
         <v>53759</v>
       </c>
-      <c r="N7">
+      <c r="N9">
         <v>118063</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P9" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q9" s="1">
         <v>45115.812395833331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10">
+        <v>447799852</v>
+      </c>
+      <c r="K10">
+        <v>11111</v>
+      </c>
+      <c r="L10">
+        <v>353</v>
+      </c>
+      <c r="M10">
+        <v>50638</v>
+      </c>
+      <c r="N10">
+        <v>117559</v>
+      </c>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>196545532</v>
+      </c>
+      <c r="K11">
+        <v>793</v>
+      </c>
+      <c r="L11">
+        <v>110</v>
+      </c>
+      <c r="M11">
+        <v>13108</v>
+      </c>
+      <c r="N11">
+        <v>58310</v>
       </c>
     </row>
   </sheetData>
@@ -794,15 +859,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10743CE8-676B-474A-8932-A83269147DD6}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1365,6 +1430,127 @@
         <v>9236</v>
       </c>
     </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>64</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>1908</v>
+      </c>
+      <c r="I10">
+        <v>1182</v>
+      </c>
+      <c r="J10">
+        <v>389</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>606</v>
+      </c>
+      <c r="M10">
+        <v>197</v>
+      </c>
+      <c r="N10">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10">
+        <v>6</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>431</v>
+      </c>
+      <c r="AD10">
+        <v>128</v>
+      </c>
+      <c r="AE10">
+        <v>105400619</v>
+      </c>
+      <c r="AF10">
+        <v>244480</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL10">
+        <v>6</v>
+      </c>
+      <c r="AM10">
+        <v>43</v>
+      </c>
+      <c r="AN10">
+        <v>5011</v>
+      </c>
+      <c r="AO10">
+        <v>9466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1375,15 +1561,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D80ED4-AEBE-471E-86CF-5C682FAEBE3C}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1946,6 +2132,127 @@
         <v>69</v>
       </c>
     </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10">
+        <v>6</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>431</v>
+      </c>
+      <c r="AD10">
+        <v>128</v>
+      </c>
+      <c r="AE10">
+        <v>52715179</v>
+      </c>
+      <c r="AF10">
+        <v>122240</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1956,15 +2263,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD22DFB-DD29-44C6-99CB-35BA0BF6DC29}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
@@ -2200,6 +2507,118 @@
       <c r="A9" t="s">
         <v>71</v>
       </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9">
+        <v>1152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9">
+        <v>431</v>
+      </c>
+      <c r="N9">
+        <v>32522398</v>
+      </c>
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" t="s">
+        <v>69</v>
+      </c>
+      <c r="U9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10">
+        <v>1152</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10">
+        <v>431</v>
+      </c>
+      <c r="N10">
+        <v>32412062</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2208,15 +2627,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE779C8C-284B-47BB-85AF-10191ACB7361}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
@@ -2452,6 +2871,118 @@
       <c r="A9" t="s">
         <v>71</v>
       </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9">
+        <v>576</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9">
+        <v>431</v>
+      </c>
+      <c r="N9">
+        <v>259462</v>
+      </c>
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" t="s">
+        <v>69</v>
+      </c>
+      <c r="U9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10">
+        <v>576</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10">
+        <v>431</v>
+      </c>
+      <c r="N10">
+        <v>258169</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2460,15 +2991,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF78D839-ACFD-4AD2-9D1B-960E83444FD8}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
   </cols>
@@ -2656,6 +3187,94 @@
       <c r="A9" t="s">
         <v>71</v>
       </c>
+      <c r="B9">
+        <v>431</v>
+      </c>
+      <c r="C9">
+        <v>431</v>
+      </c>
+      <c r="D9">
+        <v>432</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>431</v>
+      </c>
+      <c r="J9">
+        <v>432</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>113</v>
+      </c>
+      <c r="Q9">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>431</v>
+      </c>
+      <c r="C10">
+        <v>431</v>
+      </c>
+      <c r="D10">
+        <v>432</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>431</v>
+      </c>
+      <c r="J10">
+        <v>432</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>113</v>
+      </c>
+      <c r="Q10">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2664,15 +3283,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A6760C-8D41-4383-8632-7E0750667BAA}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -3000,6 +3619,80 @@
         <v>250</v>
       </c>
     </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>431</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <f>PRODUCT(C10,D10)+B10+E10</f>
+        <v>17322</v>
+      </c>
+      <c r="G10">
+        <v>41</v>
+      </c>
+      <c r="H10">
+        <v>19395</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>41</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>37</v>
+      </c>
+      <c r="W10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3007,15 +3700,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18201CF6-6FE3-47EC-9D00-A278A4489B86}">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -3412,6 +4105,91 @@
         <v>2924</v>
       </c>
     </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10">
+        <v>17240</v>
+      </c>
+      <c r="G10">
+        <v>17281</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10">
+        <v>43</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10">
+        <v>64</v>
+      </c>
+      <c r="V10">
+        <v>1106368</v>
+      </c>
+      <c r="W10" t="s">
+        <v>69</v>
+      </c>
+      <c r="X10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1690</v>
+      </c>
+      <c r="AC10">
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3419,15 +4197,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36210088-7B5A-4C26-B905-E238A58EC9C8}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="R10" sqref="R10:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -3636,6 +4414,9 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
       <c r="I8">
         <v>44</v>
       </c>
@@ -3689,6 +4470,9 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
       <c r="I9">
         <v>44</v>
       </c>
@@ -3718,6 +4502,67 @@
       </c>
       <c r="U9">
         <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10">
+        <v>1103360</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>681</v>
+      </c>
+      <c r="U10">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3727,15 +4572,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E9582-67FE-4217-8ADF-C8C533DF69AD}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -4017,10 +4862,10 @@
         <v>69</v>
       </c>
       <c r="F8">
-        <v>17240</v>
+        <v>1103360</v>
       </c>
       <c r="G8">
-        <v>17281</v>
+        <v>1103446</v>
       </c>
       <c r="H8" t="s">
         <v>69</v>
@@ -4057,6 +4902,9 @@
       </c>
       <c r="U8">
         <v>64</v>
+      </c>
+      <c r="V8" t="s">
+        <v>69</v>
       </c>
       <c r="W8">
         <v>70621248</v>
@@ -4106,10 +4954,10 @@
         <v>69</v>
       </c>
       <c r="F9">
-        <v>17240</v>
+        <v>1103360</v>
       </c>
       <c r="G9">
-        <v>17281</v>
+        <v>1103446</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
@@ -4147,6 +4995,9 @@
       <c r="U9">
         <v>64</v>
       </c>
+      <c r="V9" t="s">
+        <v>69</v>
+      </c>
       <c r="W9">
         <v>70621248</v>
       </c>
@@ -4178,6 +5029,143 @@
         <v>11912</v>
       </c>
     </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10">
+        <v>1103360</v>
+      </c>
+      <c r="G10">
+        <v>1103446</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10">
+        <v>48</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10">
+        <v>64</v>
+      </c>
+      <c r="V10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W10">
+        <v>70621184</v>
+      </c>
+      <c r="X10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>5</v>
+      </c>
+      <c r="AF10">
+        <v>3496</v>
+      </c>
+      <c r="AG10">
+        <v>10338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4185,15 +5173,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2D4F00-6636-4FBD-A21D-02274E2377D8}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:U9"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -4492,6 +5480,67 @@
         <v>353</v>
       </c>
     </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10">
+        <v>1103360</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>681</v>
+      </c>
+      <c r="U10">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4499,15 +5548,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE21D06A-FC2B-47FD-9A2A-E639A7686E88}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -4807,6 +5856,70 @@
         <v>1483</v>
       </c>
     </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10">
+        <v>551684</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>494</v>
+      </c>
+      <c r="U10">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4814,15 +5927,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3B6AB4-838F-4FAE-BEE2-C5A09D866610}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="4" width="7.140625" customWidth="1"/>
   </cols>
@@ -5104,6 +6217,67 @@
         <v>1423</v>
       </c>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10">
+        <v>27584</v>
+      </c>
+      <c r="F10">
+        <v>27600</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1216</v>
+      </c>
+      <c r="S10">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5111,15 +6285,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CABD37-21DD-4C99-A239-30AFD4E9BE66}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -5684,6 +6858,127 @@
         <v>9183</v>
       </c>
     </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>64</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>1332</v>
+      </c>
+      <c r="I10">
+        <v>606</v>
+      </c>
+      <c r="J10">
+        <v>197</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>606</v>
+      </c>
+      <c r="M10">
+        <v>197</v>
+      </c>
+      <c r="N10">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10">
+        <v>6</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>431</v>
+      </c>
+      <c r="AD10">
+        <v>64</v>
+      </c>
+      <c r="AE10">
+        <v>36826795</v>
+      </c>
+      <c r="AF10">
+        <v>85376</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL10">
+        <v>6</v>
+      </c>
+      <c r="AM10">
+        <v>43</v>
+      </c>
+      <c r="AN10">
+        <v>5008</v>
+      </c>
+      <c r="AO10">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Improved pointers calculations for conv2d and bnorm. Fixed all issues for conv2d and bnorm, that i know off.
</commit_message>
<xml_diff>
--- a/documents/HLS_microfaune_stats.xlsx
+++ b/documents/HLS_microfaune_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rodrigo\ISEL\2_Mestrado\2-ANO_1-sem\TFM\BAD_FPGA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70B5FE5-A730-4552-848A-253D3F56A0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B1551B-EF27-4F1F-B7BD-42D81413DFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{120B1578-28CF-4120-A86D-E8475CFEE8FD}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="8" xr2:uid="{120B1578-28CF-4120-A86D-E8475CFEE8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="87">
   <si>
     <t>HLS - microfaune_ai</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>results are wrong, only to explore the hw resources</t>
+  </si>
+  <si>
+    <t>fb2334b6e8369058bac73aa7a23e6c9033221754</t>
+  </si>
+  <si>
+    <t>4 ?</t>
+  </si>
+  <si>
+    <t>1 ?</t>
   </si>
 </sst>
 </file>
@@ -655,16 +664,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8BB9F6-F232-448E-BA7F-3C1C034E3083}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -824,7 +833,12 @@
       <c r="N10">
         <v>117559</v>
       </c>
-      <c r="Q10" s="1"/>
+      <c r="P10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>45117.019594907404</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -850,6 +864,12 @@
       </c>
       <c r="N11">
         <v>58310</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -861,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10743CE8-676B-474A-8932-A83269147DD6}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="Q1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +916,7 @@
     <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.5703125" customWidth="1"/>
-    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -1549,6 +1569,117 @@
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>128</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>783</v>
+      </c>
+      <c r="J11">
+        <v>256</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>399</v>
+      </c>
+      <c r="M11">
+        <v>128</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>2</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+      <c r="Z11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>431</v>
+      </c>
+      <c r="AD11">
+        <v>128</v>
+      </c>
+      <c r="AE11">
+        <v>70534443</v>
+      </c>
+      <c r="AF11">
+        <v>163584</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL11">
+        <v>6</v>
+      </c>
+      <c r="AM11">
+        <v>43</v>
+      </c>
+      <c r="AN11">
+        <v>4301</v>
+      </c>
+      <c r="AO11">
+        <v>13849</v>
       </c>
     </row>
   </sheetData>
@@ -1563,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D80ED4-AEBE-471E-86CF-5C682FAEBE3C}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1729,7 @@
     <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.5703125" customWidth="1"/>
-    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -2251,6 +2382,117 @@
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>2</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+      <c r="Z11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>431</v>
+      </c>
+      <c r="AD11">
+        <v>128</v>
+      </c>
+      <c r="AE11">
+        <v>35282091</v>
+      </c>
+      <c r="AF11">
+        <v>81792</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2265,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD22DFB-DD29-44C6-99CB-35BA0BF6DC29}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,6 +2861,57 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11">
+        <v>431</v>
+      </c>
+      <c r="N11">
+        <v>28877</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>9</v>
+      </c>
+      <c r="U11">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2630,7 +2923,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,6 +3276,57 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11">
+        <v>431</v>
+      </c>
+      <c r="N11">
+        <v>1293</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2994,7 +3338,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,6 +3619,45 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11">
+        <v>431</v>
+      </c>
+      <c r="C11">
+        <v>431</v>
+      </c>
+      <c r="D11">
+        <v>433</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>431</v>
+      </c>
+      <c r="J11">
+        <v>433</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>28</v>
+      </c>
+      <c r="Q11">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3285,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A6760C-8D41-4383-8632-7E0750667BAA}">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,6 +4075,69 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3702,8 +4148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18201CF6-6FE3-47EC-9D00-A278A4489B86}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,6 +4635,81 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" t="s">
+        <v>85</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" t="s">
+        <v>69</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4199,8 +4720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36210088-7B5A-4C26-B905-E238A58EC9C8}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R10" sqref="R10:U10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4564,6 +5085,57 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>17240</v>
+      </c>
+      <c r="E11">
+        <v>17242</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11">
+        <v>64</v>
+      </c>
+      <c r="N11">
+        <v>1103872</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>16</v>
+      </c>
+      <c r="T11">
+        <v>357</v>
+      </c>
+      <c r="U11">
+        <v>899</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4574,8 +5146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E9582-67FE-4217-8ADF-C8C533DF69AD}">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+    <sheetView topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,7 +5158,7 @@
     <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.5703125" customWidth="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5137,6 +5709,12 @@
       <c r="E11" t="s">
         <v>69</v>
       </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
       <c r="H11" t="s">
         <v>69</v>
       </c>
@@ -5146,6 +5724,9 @@
       <c r="J11" t="s">
         <v>69</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
       <c r="L11" t="s">
         <v>69</v>
       </c>
@@ -5155,6 +5736,9 @@
       <c r="N11" t="s">
         <v>69</v>
       </c>
+      <c r="O11" t="s">
+        <v>85</v>
+      </c>
       <c r="P11" t="s">
         <v>69</v>
       </c>
@@ -5162,6 +5746,42 @@
         <v>69</v>
       </c>
       <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" t="s">
+        <v>69</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5175,8 +5795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2D4F00-6636-4FBD-A21D-02274E2377D8}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,6 +6160,57 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11">
+        <v>64</v>
+      </c>
+      <c r="N11">
+        <v>1103872</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5550,8 +6221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE21D06A-FC2B-47FD-9A2A-E639A7686E88}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5887,9 +6558,6 @@
       <c r="J10" t="s">
         <v>69</v>
       </c>
-      <c r="K10" t="s">
-        <v>69</v>
-      </c>
       <c r="M10" t="s">
         <v>69</v>
       </c>
@@ -5918,6 +6586,57 @@
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11">
+        <v>551685</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>232</v>
+      </c>
+      <c r="U11">
+        <v>1324</v>
       </c>
     </row>
   </sheetData>
@@ -5929,8 +6648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3B6AB4-838F-4FAE-BEE2-C5A09D866610}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6277,6 +6996,57 @@
       <c r="A11" t="s">
         <v>80</v>
       </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>27584</v>
+      </c>
+      <c r="F11">
+        <v>27595</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>610</v>
+      </c>
+      <c r="S11">
+        <v>1043</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6287,8 +7057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CABD37-21DD-4C99-A239-30AFD4E9BE66}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6322,6 +7092,7 @@
     <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.5703125" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -6977,6 +7748,117 @@
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>399</v>
+      </c>
+      <c r="J11">
+        <v>128</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>399</v>
+      </c>
+      <c r="M11">
+        <v>128</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <v>2</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+      <c r="Z11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>431</v>
+      </c>
+      <c r="AD11">
+        <v>64</v>
+      </c>
+      <c r="AE11">
+        <v>24689835</v>
+      </c>
+      <c r="AF11">
+        <v>57216</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL11">
+        <v>6</v>
+      </c>
+      <c r="AM11">
+        <v>43</v>
+      </c>
+      <c r="AN11">
+        <v>4314</v>
+      </c>
+      <c r="AO11">
+        <v>13794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>